<commit_message>
Burndown Chart Commit by P.D
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -52,15 +52,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="175" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -68,7 +68,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -77,7 +77,7 @@
       <i/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -235,7 +235,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -244,7 +244,7 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="175" formatCode="0.0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -456,7 +456,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -521,7 +521,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fa-IR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -615,25 +615,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.428571428571429</c:v>
+                  <c:v>20.571428571428573</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.857142857142858</c:v>
+                  <c:v>17.142857142857146</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.285714285714286</c:v>
+                  <c:v>13.714285714285717</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.7142857142857153</c:v>
+                  <c:v>10.285714285714288</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1428571428571441</c:v>
+                  <c:v>6.8571428571428594</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5714285714285725</c:v>
+                  <c:v>3.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -642,6 +642,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-396D-4C32-AF55-9E397447B2BE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -727,25 +732,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -754,6 +759,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-396D-4C32-AF55-9E397447B2BE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -839,7 +849,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fa-IR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -877,7 +887,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fa-IR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="318087008"/>
@@ -962,7 +972,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fa-IR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1000,7 +1010,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fa-IR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="318081128"/>
@@ -1043,7 +1053,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fa-IR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1073,7 +1083,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fa-IR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1948,17 +1958,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1967,7 +1977,7 @@
       </c>
       <c r="B1" s="9">
         <f>SUM(Table1[Total Actual Daily Effort])</f>
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1984,7 +1994,7 @@
       </c>
       <c r="B3" s="9">
         <f>B1/B2</f>
-        <v>2.5714285714285716</v>
+        <v>3.4285714285714284</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2031,20 +2041,18 @@
       </c>
       <c r="F7" s="5">
         <f>B1</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G7" s="10">
         <f>B1</f>
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
+      <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5">
@@ -2053,11 +2061,11 @@
       </c>
       <c r="F8" s="5">
         <f>F7-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G8" s="10">
         <f>G7-B$3</f>
-        <v>15.428571428571429</v>
+        <v>20.571428571428573</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2073,11 +2081,11 @@
       </c>
       <c r="F9" s="5">
         <f>F8-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G9" s="10">
         <f t="shared" ref="G9:G14" si="0">G8-B$3</f>
-        <v>12.857142857142858</v>
+        <v>17.142857142857146</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2093,11 +2101,11 @@
       </c>
       <c r="F10" s="5">
         <f>F9-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G10" s="10">
         <f t="shared" si="0"/>
-        <v>10.285714285714286</v>
+        <v>13.714285714285717</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2113,11 +2121,11 @@
       </c>
       <c r="F11" s="5">
         <f>F10-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G11" s="10">
         <f t="shared" si="0"/>
-        <v>7.7142857142857153</v>
+        <v>10.285714285714288</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2125,9 +2133,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5">
         <f>SUM(Table1[[#This Row],[Member 1]:[Member 3]])</f>
@@ -2135,11 +2141,11 @@
       </c>
       <c r="F12" s="5">
         <f>F11-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G12" s="10">
         <f t="shared" si="0"/>
-        <v>5.1428571428571441</v>
+        <v>6.8571428571428594</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2152,18 +2158,20 @@
       <c r="C13" s="5">
         <v>3</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
       <c r="E13" s="5">
         <f>SUM(Table1[[#This Row],[Member 1]:[Member 3]])</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F13" s="5">
         <f>F12-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G13" s="10">
         <f t="shared" si="0"/>
-        <v>2.5714285714285725</v>
+        <v>3.428571428571431</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2176,10 +2184,12 @@
       <c r="C14" s="7">
         <v>4</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7">
+        <v>4</v>
+      </c>
       <c r="E14" s="7">
         <f>SUM(Table1[[#This Row],[Member 1]:[Member 3]])</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F14" s="5">
         <f>F13-Table1[[#This Row],[Total Actual Daily Effort]]</f>

</xml_diff>

<commit_message>
Parsa Committed BurnDown Chart
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="6492"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -60,7 +60,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -68,7 +68,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -77,7 +77,7 @@
       <i/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -456,7 +456,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -521,7 +521,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fa-IR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -615,25 +615,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.142857142857142</c:v>
+                  <c:v>34.285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.285714285714285</c:v>
+                  <c:v>28.571428571428569</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.428571428571427</c:v>
+                  <c:v>22.857142857142854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.571428571428569</c:v>
+                  <c:v>17.142857142857139</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.7142857142857117</c:v>
+                  <c:v>11.428571428571423</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8571428571428545</c:v>
+                  <c:v>5.7142857142857091</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -642,7 +642,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-396D-4C32-AF55-9E397447B2BE}"/>
             </c:ext>
@@ -732,25 +732,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -759,7 +759,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-396D-4C32-AF55-9E397447B2BE}"/>
             </c:ext>
@@ -849,7 +849,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fa-IR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -887,7 +887,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fa-IR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="337905672"/>
@@ -972,7 +972,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fa-IR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1010,7 +1010,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fa-IR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="337905280"/>
@@ -1053,7 +1053,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fa-IR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1083,7 +1083,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fa-IR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1959,16 +1959,16 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
       </c>
       <c r="B1" s="9">
         <f>SUM(Table1[Total Actual Daily Effort])</f>
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="B3" s="9">
         <f>B1/B2</f>
-        <v>3.8571428571428572</v>
+        <v>5.7142857142857144</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2041,11 +2041,11 @@
       </c>
       <c r="F7" s="5">
         <f>B1</f>
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G7" s="10">
         <f>B1</f>
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2061,11 +2061,11 @@
       </c>
       <c r="F8" s="5">
         <f>F7-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G8" s="10">
         <f>G7-B$3</f>
-        <v>23.142857142857142</v>
+        <v>34.285714285714285</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2083,11 +2083,11 @@
       </c>
       <c r="F9" s="5">
         <f>F8-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G9" s="10">
         <f t="shared" ref="G9:G14" si="0">G8-B$3</f>
-        <v>19.285714285714285</v>
+        <v>28.571428571428569</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2105,11 +2105,11 @@
       </c>
       <c r="F10" s="5">
         <f>F9-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G10" s="10">
         <f t="shared" si="0"/>
-        <v>15.428571428571427</v>
+        <v>22.857142857142854</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2118,18 +2118,20 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
       <c r="E11" s="5">
         <f>SUM(Table1[[#This Row],[Member 1]:[Member 3]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="5">
         <f>F10-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G11" s="10">
         <f t="shared" si="0"/>
-        <v>11.571428571428569</v>
+        <v>17.142857142857139</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2140,18 +2142,20 @@
         <v>10</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5">
+        <v>2</v>
+      </c>
       <c r="E12" s="5">
         <f>SUM(Table1[[#This Row],[Member 1]:[Member 3]])</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F12" s="5">
         <f>F11-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G12" s="10">
         <f t="shared" si="0"/>
-        <v>7.7142857142857117</v>
+        <v>11.428571428571423</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2162,18 +2166,20 @@
         <v>10</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5">
+        <v>5</v>
+      </c>
       <c r="E13" s="5">
         <f>SUM(Table1[[#This Row],[Member 1]:[Member 3]])</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F13" s="5">
         <f>F12-Table1[[#This Row],[Total Actual Daily Effort]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G13" s="10">
         <f t="shared" si="0"/>
-        <v>3.8571428571428545</v>
+        <v>5.7142857142857091</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2184,10 +2190,12 @@
         <v>0</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7">
+        <v>5</v>
+      </c>
       <c r="E14" s="7">
         <f>SUM(Table1[[#This Row],[Member 1]:[Member 3]])</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F14" s="5">
         <f>F13-Table1[[#This Row],[Total Actual Daily Effort]]</f>

</xml_diff>